<commit_message>
data for line chart init
</commit_message>
<xml_diff>
--- a/project log.xlsx
+++ b/project log.xlsx
@@ -14,16 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>obj</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>approach</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,10 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>unsolved prob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>can't make the scrollbar identical to browzer's default scrollbar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,15 +148,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>found bug in dataparsing process</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>found out that although I tried to make a copy of the origin data then process the copy, I was modifiying the original data, since the elements in the data array are objs. So I was passing reference to the copy.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>since console.log() is asynchronous, it gets fired after the main body of the function is completed, the printed result is not the result at the expected moment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug in dataparsing for graph3 and 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to be fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searched online, found a way of using JSON.parse(JSON.stringify(array)) to deep copy array of objs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj/prob encountered</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed data in graph3 and 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">found duplication in rawdata, wonder whether need to deduplicate. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dedup in the future</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed data fetching with fake data in chart2, all four charts are displayed with fake data now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug with stacking feature in the library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compared with demo code, tried different approaches to solve the prob. At last, got answer from the library team that it is the bug in the library that leads to the issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maybe need to change the way from fetching from dataset to extract data and fetch into series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>follow up</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -537,13 +573,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
@@ -551,51 +587,39 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
@@ -603,40 +627,31 @@
         <v>1.17</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1.17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1.17</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1.17</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
@@ -644,57 +659,45 @@
         <v>1.18</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
@@ -702,39 +705,79 @@
         <v>1.19</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1.19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1.2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="86.4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes and doc updates
</commit_message>
<xml_diff>
--- a/project log.xlsx
+++ b/project log.xlsx
@@ -10,11 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,99 +109,181 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>change the data input method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found it not convinient to write data into series, learned dataset using reference, change data interface format into array of arrays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>went through apis and examples, failed to make the axis response to click. Create buttons at the bottom instead to control  sorting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ask whether the visulization is acceptable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajax dataloading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">decided to upload csv to github to use ajax request. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataparsing for chart3 and 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>restructured Dom, added chart4 in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found out that although I tried to make a copy of the origin data then process the copy, I was modifiying the original data, since the elements in the data array are objs. So I was passing reference to the copy.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>since console.log() is asynchronous, it gets fired after the main body of the function is completed, the printed result is not the result at the expected moment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug in dataparsing for graph3 and 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to be fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searched online, found a way of using JSON.parse(JSON.stringify(array)) to deep copy array of objs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj/prob encountered</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed data in graph3 and 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">found duplication in rawdata, wonder whether need to deduplicate. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dedup in the future</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed data fetching with fake data in chart2, all four charts are displayed with fake data now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug with stacking feature in the library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>compared with demo code, tried different approaches to solve the prob. At last, got answer from the library team that it is the bug in the library that leads to the issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maybe need to change the way from fetching from dataset to extract data and fetch into series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>adjust layout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>change the data input method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>found it not convinient to write data into series, learned dataset using reference, change data interface format into array of arrays</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>axis and text position can't be adjusted</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>went through apis and examples, failed to make the axis response to click. Create buttons at the bottom instead to control  sorting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ask whether the visulization is acceptable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ajax dataloading</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">decided to upload csv to github to use ajax request. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dataparsing for chart3 and 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>restructured Dom, added chart4 in</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>found out that although I tried to make a copy of the origin data then process the copy, I was modifiying the original data, since the elements in the data array are objs. So I was passing reference to the copy.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>since console.log() is asynchronous, it gets fired after the main body of the function is completed, the printed result is not the result at the expected moment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>found bug in dataparsing for graph3 and 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>to be fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>searched online, found a way of using JSON.parse(JSON.stringify(array)) to deep copy array of objs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>obj/prob encountered</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed data in graph3 and 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">found duplication in rawdata, wonder whether need to deduplicate. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dedup in the future</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed data fetching with fake data in chart2, all four charts are displayed with fake data now</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>found bug with stacking feature in the library</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>compared with demo code, tried different approaches to solve the prob. At last, got answer from the library team that it is the bug in the library that leads to the issue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maybe need to change the way from fetching from dataset to extract data and fetch into series</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>follow up</t>
+    <t>get stuck with processing data for drill up/down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>went through moment.js's api, tried different methods, finally came up with a reusable drilltime function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug in drilltime func</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>after filtering result, tracking breakpoint, found it is the edge case of checking whether the time falls in the range caused the prob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>working with date obj api, searching for method for grouping data according to time dimension</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>too complicated to calculate time range and start/end point for new grouped data's time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit axis label and tooltip for line charts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>further action needed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adjust yaxis label and layout to match layout of given bar charts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis and label text position can't be adjusted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found out that can use grid option to adjust yaxis and label text position for barcharts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrote linesplitter function to format the yaxis label for bar charts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expolored way to select elem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tried click event and brush, finally, chose to use brush to select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrote button with event listener to keep/remove selected data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found bug with dataset in dataView component</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reformat dataview to show the data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>used a module called moment.js to calculate duration and time point for grouped data
+data process completed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>format tooltip for all the charts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the param of idx passed into linecharts is empty
+can't scroll to select with the datazoom bar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switched to yaxis brush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>found library bug with square brush</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -208,7 +291,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +301,21 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -244,12 +342,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -554,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -573,13 +677,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
@@ -673,7 +777,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
@@ -681,23 +785,23 @@
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
@@ -705,15 +809,15 @@
         <v>1.19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
@@ -721,23 +825,23 @@
         <v>1.2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="86.4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
@@ -745,39 +849,139 @@
         <v>1.21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1.22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>1.26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>